<commit_message>
now health benefits update
</commit_message>
<xml_diff>
--- a/Input/Now_Health/Old/benefits1.xlsx
+++ b/Input/Now_Health/Old/benefits1.xlsx
@@ -545,11 +545,11 @@
   </sheetPr>
   <dimension ref="A1:BM10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BC1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BH3" activeCellId="0" sqref="BH3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.49"/>
@@ -801,7 +801,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>62</v>
       </c>
@@ -946,10 +946,10 @@
         <v>89</v>
       </c>
       <c r="BG2" s="7" t="n">
-        <v>45017</v>
+        <v>45383</v>
       </c>
       <c r="BH2" s="8" t="n">
-        <v>45382</v>
+        <v>45747</v>
       </c>
       <c r="BI2" s="0" t="s">
         <v>90</v>
@@ -967,7 +967,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>102</v>
       </c>
@@ -1270,7 +1270,7 @@
       <c r="BH4" s="8"/>
       <c r="BJ4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>105</v>
       </c>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="BJ5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>113</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="BJ6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>114</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>115</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>122</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>123</v>
       </c>

</xml_diff>